<commit_message>
Added Gothic transect data.
</commit_message>
<xml_diff>
--- a/bombus_data.xlsx
+++ b/bombus_data.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Proboscis lengths" sheetId="2" r:id="rId1"/>
     <sheet name="Proboscis and corolla lengths" sheetId="3" r:id="rId2"/>
     <sheet name="Flower visits" sheetId="1" r:id="rId3"/>
-    <sheet name="Washington transect" sheetId="4" r:id="rId4"/>
-    <sheet name="Schofield transect" sheetId="5" r:id="rId5"/>
+    <sheet name="Gothic transect" sheetId="6" r:id="rId4"/>
+    <sheet name="Washington transect" sheetId="4" r:id="rId5"/>
+    <sheet name="Schofield transect" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>Delphinium nelsoni</t>
   </si>
@@ -172,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,6 +184,38 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -205,16 +238,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,7 +532,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -502,19 +544,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1642,7 +1684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1656,19 +1700,19 @@
       <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2248,9 +2292,386 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.88</v>
+      </c>
+      <c r="E2">
+        <v>0.02</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.91</v>
+      </c>
+      <c r="E3">
+        <v>0.01</v>
+      </c>
+      <c r="F3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.99</v>
+      </c>
+      <c r="C4">
+        <v>0.01</v>
+      </c>
+      <c r="D4">
+        <v>0.94</v>
+      </c>
+      <c r="E4">
+        <v>0.03</v>
+      </c>
+      <c r="F4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.88</v>
+      </c>
+      <c r="E5">
+        <v>0.05</v>
+      </c>
+      <c r="F5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.69</v>
+      </c>
+      <c r="E6">
+        <v>0.15</v>
+      </c>
+      <c r="F6">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.97</v>
+      </c>
+      <c r="C7">
+        <v>0.03</v>
+      </c>
+      <c r="D7">
+        <v>0.68</v>
+      </c>
+      <c r="E7">
+        <v>0.25</v>
+      </c>
+      <c r="F7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.98</v>
+      </c>
+      <c r="C8">
+        <v>0.02</v>
+      </c>
+      <c r="D8">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E8">
+        <v>0.38</v>
+      </c>
+      <c r="F8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.93</v>
+      </c>
+      <c r="C9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.47</v>
+      </c>
+      <c r="E9">
+        <v>0.32</v>
+      </c>
+      <c r="F9">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.91</v>
+      </c>
+      <c r="C10">
+        <v>0.09</v>
+      </c>
+      <c r="D10">
+        <v>0.42</v>
+      </c>
+      <c r="E10">
+        <v>0.44</v>
+      </c>
+      <c r="F10">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.97</v>
+      </c>
+      <c r="C11">
+        <v>0.03</v>
+      </c>
+      <c r="D11">
+        <v>0.17</v>
+      </c>
+      <c r="E11">
+        <v>0.49</v>
+      </c>
+      <c r="F11">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E12">
+        <v>0.59</v>
+      </c>
+      <c r="F12">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0.82</v>
+      </c>
+      <c r="C13">
+        <v>0.18</v>
+      </c>
+      <c r="D13">
+        <v>0.45</v>
+      </c>
+      <c r="E13">
+        <v>0.22</v>
+      </c>
+      <c r="F13">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0.51</v>
+      </c>
+      <c r="C14">
+        <v>0.49</v>
+      </c>
+      <c r="D14">
+        <v>0.04</v>
+      </c>
+      <c r="E14">
+        <v>0.26</v>
+      </c>
+      <c r="F14">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0.67</v>
+      </c>
+      <c r="C15">
+        <v>0.33</v>
+      </c>
+      <c r="D15">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E15">
+        <v>0.09</v>
+      </c>
+      <c r="F15">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.4</v>
+      </c>
+      <c r="C16">
+        <v>0.6</v>
+      </c>
+      <c r="D16">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E16">
+        <v>0.11</v>
+      </c>
+      <c r="F16">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0.16</v>
+      </c>
+      <c r="C17">
+        <v>0.84</v>
+      </c>
+      <c r="D17">
+        <v>0.05</v>
+      </c>
+      <c r="E17">
+        <v>0.17</v>
+      </c>
+      <c r="F17">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0.02</v>
+      </c>
+      <c r="C18">
+        <v>0.98</v>
+      </c>
+      <c r="D18">
+        <v>0.12</v>
+      </c>
+      <c r="E18">
+        <v>0.15</v>
+      </c>
+      <c r="F18">
+        <v>0.73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2439,7 +2860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Deleted Washington and Schofield transects.
</commit_message>
<xml_diff>
--- a/bombus_data.xlsx
+++ b/bombus_data.xlsx
@@ -9,15 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Proboscis lengths" sheetId="2" r:id="rId1"/>
     <sheet name="Proboscis and corolla lengths" sheetId="3" r:id="rId2"/>
     <sheet name="Flower visits" sheetId="1" r:id="rId3"/>
     <sheet name="Gothic transect" sheetId="6" r:id="rId4"/>
-    <sheet name="Washington transect" sheetId="4" r:id="rId5"/>
-    <sheet name="Schofield transect" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Delphinium nelsoni</t>
   </si>
@@ -243,11 +241,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -532,9 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -544,19 +538,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1684,9 +1678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1700,19 +1692,19 @@
       <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2294,597 +2286,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0.88</v>
-      </c>
-      <c r="E2">
-        <v>0.02</v>
-      </c>
-      <c r="F2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0.91</v>
-      </c>
-      <c r="E3">
-        <v>0.01</v>
-      </c>
-      <c r="F3">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0.99</v>
-      </c>
-      <c r="C4">
-        <v>0.01</v>
-      </c>
-      <c r="D4">
-        <v>0.94</v>
-      </c>
-      <c r="E4">
-        <v>0.03</v>
-      </c>
-      <c r="F4">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0.88</v>
-      </c>
-      <c r="E5">
-        <v>0.05</v>
-      </c>
-      <c r="F5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0.69</v>
-      </c>
-      <c r="E6">
-        <v>0.15</v>
-      </c>
-      <c r="F6">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0.97</v>
-      </c>
-      <c r="C7">
-        <v>0.03</v>
-      </c>
-      <c r="D7">
-        <v>0.68</v>
-      </c>
-      <c r="E7">
-        <v>0.25</v>
-      </c>
-      <c r="F7">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0.98</v>
-      </c>
-      <c r="C8">
-        <v>0.02</v>
-      </c>
-      <c r="D8">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="E8">
-        <v>0.38</v>
-      </c>
-      <c r="F8">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0.93</v>
-      </c>
-      <c r="C9">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D9">
-        <v>0.47</v>
-      </c>
-      <c r="E9">
-        <v>0.32</v>
-      </c>
-      <c r="F9">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0.91</v>
-      </c>
-      <c r="C10">
-        <v>0.09</v>
-      </c>
-      <c r="D10">
-        <v>0.42</v>
-      </c>
-      <c r="E10">
-        <v>0.44</v>
-      </c>
-      <c r="F10">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>0.97</v>
-      </c>
-      <c r="C11">
-        <v>0.03</v>
-      </c>
-      <c r="D11">
-        <v>0.17</v>
-      </c>
-      <c r="E11">
-        <v>0.49</v>
-      </c>
-      <c r="F11">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E12">
-        <v>0.59</v>
-      </c>
-      <c r="F12">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>0.82</v>
-      </c>
-      <c r="C13">
-        <v>0.18</v>
-      </c>
-      <c r="D13">
-        <v>0.45</v>
-      </c>
-      <c r="E13">
-        <v>0.22</v>
-      </c>
-      <c r="F13">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0.51</v>
-      </c>
-      <c r="C14">
-        <v>0.49</v>
-      </c>
-      <c r="D14">
-        <v>0.04</v>
-      </c>
-      <c r="E14">
-        <v>0.26</v>
-      </c>
-      <c r="F14">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0.67</v>
-      </c>
-      <c r="C15">
-        <v>0.33</v>
-      </c>
-      <c r="D15">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E15">
-        <v>0.09</v>
-      </c>
-      <c r="F15">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>0.4</v>
-      </c>
-      <c r="C16">
-        <v>0.6</v>
-      </c>
-      <c r="D16">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E16">
-        <v>0.11</v>
-      </c>
-      <c r="F16">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>0.16</v>
-      </c>
-      <c r="C17">
-        <v>0.84</v>
-      </c>
-      <c r="D17">
-        <v>0.05</v>
-      </c>
-      <c r="E17">
-        <v>0.17</v>
-      </c>
-      <c r="F17">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>0.02</v>
-      </c>
-      <c r="C18">
-        <v>0.98</v>
-      </c>
-      <c r="D18">
-        <v>0.12</v>
-      </c>
-      <c r="E18">
-        <v>0.15</v>
-      </c>
-      <c r="F18">
-        <v>0.73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.62</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.96</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.73</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.86</v>
-      </c>
-      <c r="F4" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.88</v>
-      </c>
-      <c r="F5" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.33</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.71</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.37</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.63</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.37</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.63</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.54</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.37</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.63</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.31</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.69</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2892,120 +2314,340 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.11</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.33</v>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.88</v>
+      </c>
+      <c r="E2">
+        <v>0.02</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.91</v>
+      </c>
+      <c r="E3">
+        <v>0.01</v>
+      </c>
+      <c r="F3">
         <v>0.08</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.92</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.64</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.84</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.21</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.49</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.3</v>
+      <c r="B4">
+        <v>0.99</v>
+      </c>
+      <c r="C4">
+        <v>0.01</v>
+      </c>
+      <c r="D4">
+        <v>0.94</v>
+      </c>
+      <c r="E4">
+        <v>0.03</v>
+      </c>
+      <c r="F4">
+        <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.88</v>
+      </c>
+      <c r="E5">
+        <v>0.05</v>
+      </c>
+      <c r="F5">
         <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.93</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.34</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.54</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.98</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.64</v>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.69</v>
+      </c>
+      <c r="E6">
+        <v>0.15</v>
+      </c>
+      <c r="F6">
+        <v>0.16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
+        <v>0.97</v>
+      </c>
+      <c r="C7">
+        <v>0.03</v>
+      </c>
+      <c r="D7">
+        <v>0.68</v>
+      </c>
+      <c r="E7">
+        <v>0.25</v>
+      </c>
+      <c r="F7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.98</v>
+      </c>
+      <c r="C8">
+        <v>0.02</v>
+      </c>
+      <c r="D8">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E8">
+        <v>0.38</v>
+      </c>
+      <c r="F8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.93</v>
+      </c>
+      <c r="C9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.47</v>
+      </c>
+      <c r="E9">
+        <v>0.32</v>
+      </c>
+      <c r="F9">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.91</v>
+      </c>
+      <c r="C10">
+        <v>0.09</v>
+      </c>
+      <c r="D10">
+        <v>0.42</v>
+      </c>
+      <c r="E10">
+        <v>0.44</v>
+      </c>
+      <c r="F10">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.97</v>
+      </c>
+      <c r="C11">
+        <v>0.03</v>
+      </c>
+      <c r="D11">
+        <v>0.17</v>
+      </c>
+      <c r="E11">
+        <v>0.49</v>
+      </c>
+      <c r="F11">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>0</v>
       </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="D12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E12">
+        <v>0.59</v>
+      </c>
+      <c r="F12">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0.82</v>
+      </c>
+      <c r="C13">
+        <v>0.18</v>
+      </c>
+      <c r="D13">
+        <v>0.45</v>
+      </c>
+      <c r="E13">
+        <v>0.22</v>
+      </c>
+      <c r="F13">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0.51</v>
+      </c>
+      <c r="C14">
+        <v>0.49</v>
+      </c>
+      <c r="D14">
         <v>0.04</v>
       </c>
-      <c r="E7" s="3">
-        <v>0.24</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.72</v>
+      <c r="E14">
+        <v>0.26</v>
+      </c>
+      <c r="F14">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0.67</v>
+      </c>
+      <c r="C15">
+        <v>0.33</v>
+      </c>
+      <c r="D15">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E15">
+        <v>0.09</v>
+      </c>
+      <c r="F15">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.4</v>
+      </c>
+      <c r="C16">
+        <v>0.6</v>
+      </c>
+      <c r="D16">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E16">
+        <v>0.11</v>
+      </c>
+      <c r="F16">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0.16</v>
+      </c>
+      <c r="C17">
+        <v>0.84</v>
+      </c>
+      <c r="D17">
+        <v>0.05</v>
+      </c>
+      <c r="E17">
+        <v>0.17</v>
+      </c>
+      <c r="F17">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0.02</v>
+      </c>
+      <c r="C18">
+        <v>0.98</v>
+      </c>
+      <c r="D18">
+        <v>0.12</v>
+      </c>
+      <c r="E18">
+        <v>0.15</v>
+      </c>
+      <c r="F18">
+        <v>0.73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>